<commit_message>
Updated Status for 3/1/18 morning
</commit_message>
<xml_diff>
--- a/work_done.xlsx
+++ b/work_done.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>28.12.17</t>
   </si>
@@ -86,9 +86,6 @@
     <t>absent</t>
   </si>
   <si>
-    <t>2.1.18</t>
-  </si>
-  <si>
     <t>Updating Fields in Application</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>11:00 to 14:30</t>
   </si>
   <si>
-    <t>SRIRAM</t>
-  </si>
-  <si>
     <t>14:00 to 16:00</t>
   </si>
   <si>
@@ -111,13 +105,45 @@
   </si>
   <si>
     <t>56% Completed</t>
+  </si>
+  <si>
+    <t>11:00 to 12:00</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Automated application login and scrape data fetched from database. Written those scraped data into a csv file using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>write csv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> activity</t>
+    </r>
+  </si>
+  <si>
+    <t>28-12-2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +168,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -191,7 +225,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -200,8 +234,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -567,104 +608,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="40.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8">
+        <v>43132</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="E6" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8">
+        <v>43160</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>27</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F4">
+  <conditionalFormatting sqref="E4">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"""in progress"""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Status update for 4-1-18
</commit_message>
<xml_diff>
--- a/work_done.xlsx
+++ b/work_done.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>28.12.17</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>14:00 to 16:00</t>
-  </si>
-  <si>
-    <t>UiPath Course</t>
   </si>
   <si>
     <t>56% Completed</t>
@@ -136,7 +133,10 @@
     </r>
   </si>
   <si>
-    <t>28-12-2017</t>
+    <t>75% Completed</t>
+  </si>
+  <si>
+    <t>UiPath Course - 1</t>
   </si>
 </sst>
 </file>
@@ -225,7 +225,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -243,6 +243,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -608,10 +614,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,20 +633,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -648,8 +654,8 @@
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>28</v>
+      <c r="B4" s="8">
+        <v>43462</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>21</v>
@@ -666,7 +672,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="8">
-        <v>43132</v>
+        <v>43102</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>22</v>
@@ -685,10 +691,10 @@
         <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -696,16 +702,33 @@
         <v>3</v>
       </c>
       <c r="B7" s="8">
-        <v>43160</v>
+        <v>43103</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" s="9">
+        <v>43104</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Task - 8-1 F/N
</commit_message>
<xml_diff>
--- a/work_done.xlsx
+++ b/work_done.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
   <si>
     <t>28.12.17</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>UiPath Course - 1</t>
+  </si>
+  <si>
+    <t>11:30 to 13:30</t>
+  </si>
+  <si>
+    <t>Completed UiPATH course and obtained Certificate</t>
   </si>
 </sst>
 </file>
@@ -225,7 +231,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -249,6 +255,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -614,10 +621,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,6 +736,23 @@
       </c>
       <c r="E8" s="12" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" s="9">
+        <v>43108</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working model on 26/3/18
</commit_message>
<xml_diff>
--- a/work_done.xlsx
+++ b/work_done.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="74">
   <si>
     <t>28.12.17</t>
   </si>
@@ -245,6 +245,33 @@
   </si>
   <si>
     <t>EXAM</t>
+  </si>
+  <si>
+    <t>Created forms and tried to push values to database through forms</t>
+  </si>
+  <si>
+    <t>automated data update in database through forms</t>
+  </si>
+  <si>
+    <t>Found bugs in data entry and trying to resolve it</t>
+  </si>
+  <si>
+    <t>Found alternative method for pushing data to database through build data table</t>
+  </si>
+  <si>
+    <t>Implemented build datatable method for data pushing</t>
+  </si>
+  <si>
+    <t>Found errors in pushing data</t>
+  </si>
+  <si>
+    <t>Trying to resolve bugs</t>
+  </si>
+  <si>
+    <t>Resolved bugs</t>
+  </si>
+  <si>
+    <t>Integrating project and debugging</t>
   </si>
 </sst>
 </file>
@@ -738,10 +765,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1218,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="9">
         <v>43157</v>
       </c>
@@ -1199,7 +1226,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="9">
         <v>43158</v>
       </c>
@@ -1207,7 +1234,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="9">
         <v>43159</v>
       </c>
@@ -1215,7 +1242,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="9">
         <v>43160</v>
       </c>
@@ -1223,7 +1250,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="9">
         <v>43161</v>
       </c>
@@ -1231,7 +1258,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="9">
         <v>43162</v>
       </c>
@@ -1239,7 +1266,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="9">
         <v>43163</v>
       </c>
@@ -1247,7 +1274,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="9">
         <v>43164</v>
       </c>
@@ -1255,7 +1282,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="9">
         <v>43165</v>
       </c>
@@ -1263,12 +1290,180 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="9">
         <v>43166</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="9">
+        <v>43167</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="9">
+        <v>43168</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B45" s="9">
+        <v>43170</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="9">
+        <v>43171</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="9">
+        <v>43172</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="9">
+        <v>43173</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B49" s="9">
+        <v>43174</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="9">
+        <v>43175</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="9">
+        <v>43176</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="9">
+        <v>43177</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="9">
+        <v>43178</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E53" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="9">
+        <v>43179</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="9">
+        <v>43180</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="9">
+        <v>43181</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="9">
+        <v>43182</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="9">
+        <v>43183</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="9">
+        <v>43184</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="9">
+        <v>43185</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>